<commit_message>
cambios de may 2do vobo final
</commit_message>
<xml_diff>
--- a/xlsx/a69_f02_aUPPachuca.xlsx
+++ b/xlsx/a69_f02_aUPPachuca.xlsx
@@ -5,21 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dirección de Planeción\2022\SIPOT\UPP 2DO TRI 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sala5\Documents\UPP Solvetacion de Observaciones 1er  Vo. Bo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="179">
   <si>
     <t>43962</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Nota</t>
   </si>
   <si>
-    <t>Recursos Humanos (UPP)</t>
-  </si>
-  <si>
     <t>Rectoría</t>
   </si>
   <si>
@@ -210,6 +207,15 @@
     <t>Artículos 27 y 31 del Estatuto Orgánico de la Universidad Politécnica de Pachuca</t>
   </si>
   <si>
+    <t>Órgano Interno de Control</t>
+  </si>
+  <si>
+    <t>Titular del Órgano Interno de Control</t>
+  </si>
+  <si>
+    <t>Artículos 27 y 79 del Estatuto Orgánico de la Universidad Politécnica de Pachuca</t>
+  </si>
+  <si>
     <t>Dirección de Vinculación y Extensión</t>
   </si>
   <si>
@@ -546,26 +552,17 @@
     <t>Jefa de Departamento de Evaluación y Estadísticas</t>
   </si>
   <si>
-    <t>Los prestadores de servicios profesionales no forman parte de la estructura orgánica de la institución.</t>
-  </si>
-  <si>
-    <t>Órgano Interno de Control</t>
-  </si>
-  <si>
-    <t>Titular del Órgano Interno de Control</t>
-  </si>
-  <si>
-    <t>Artículos 27 y 79 del Estatuto Orgánico de la Universidad Politécnica de Pachuca</t>
-  </si>
-  <si>
     <t>La plaza del Titular del Órgano Interno de Control, dejó de pertenecer a la Estructura de la Universidad, y pasó a la Secretaría de Contraloría a partir del 16 de enero 2022.</t>
+  </si>
+  <si>
+    <t>Departamento de Recursos Humanos (UPP)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -594,8 +591,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -619,7 +622,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -642,6 +645,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -650,7 +664,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -667,33 +681,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -977,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L2" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,18 +988,18 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="111.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="87.7109375" customWidth="1"/>
+    <col min="10" max="10" width="93.5703125" customWidth="1"/>
     <col min="11" max="11" width="47.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="65" customWidth="1"/>
+    <col min="15" max="15" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1006,38 +1008,38 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="13" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1134,23 +1136,23 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1204,228 +1206,226 @@
         <v>2022</v>
       </c>
       <c r="B8" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C8" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>45</v>
+      <c r="L8" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M8" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N8" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O8" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2022</v>
       </c>
       <c r="B9" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C9" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K9" s="2">
-        <v>1</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>45</v>
+        <v>0</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M9" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N9" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>175</v>
-      </c>
+        <v>44844</v>
+      </c>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2022</v>
       </c>
       <c r="B10" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C10" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="I10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>45</v>
+      <c r="L10" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M10" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N10" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O10" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2022</v>
       </c>
       <c r="B11" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C11" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="M11" s="3">
+        <v>44844</v>
+      </c>
+      <c r="N11" s="3">
+        <v>44844</v>
+      </c>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44743</v>
+      </c>
+      <c r="C12" s="3">
+        <v>44834</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="M11" s="3">
-        <v>44753</v>
-      </c>
-      <c r="N11" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B12" s="9">
-        <v>44652</v>
-      </c>
-      <c r="C12" s="9">
-        <v>44742</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="E12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="3">
+        <v>44844</v>
+      </c>
+      <c r="N12" s="3">
+        <v>44844</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="M12" s="9">
-        <v>44753</v>
-      </c>
-      <c r="N12" s="9">
-        <v>44753</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -1433,2162 +1433,2160 @@
         <v>2022</v>
       </c>
       <c r="B13" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C13" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>45</v>
+      <c r="L13" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M13" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N13" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O13" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2022</v>
       </c>
       <c r="B14" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C14" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K14" s="2">
         <v>0</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>45</v>
+      <c r="L14" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M14" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N14" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O14" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O14" s="6"/>
     </row>
     <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2022</v>
       </c>
       <c r="B15" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C15" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>45</v>
+      <c r="L15" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M15" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N15" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2022</v>
       </c>
       <c r="B16" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C16" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K16" s="2">
         <v>0</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>45</v>
+      <c r="L16" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M16" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N16" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2022</v>
       </c>
       <c r="B17" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C17" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K17" s="2">
-        <v>1</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>45</v>
+        <v>0</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M17" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N17" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>175</v>
-      </c>
+        <v>44844</v>
+      </c>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2022</v>
       </c>
       <c r="B18" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C18" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K18" s="2">
         <v>0</v>
       </c>
-      <c r="L18" s="6" t="s">
-        <v>45</v>
+      <c r="L18" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M18" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N18" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O18" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O18" s="6"/>
     </row>
     <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2022</v>
       </c>
       <c r="B19" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C19" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K19" s="2">
         <v>0</v>
       </c>
-      <c r="L19" s="6" t="s">
-        <v>45</v>
+      <c r="L19" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M19" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N19" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O19" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O19" s="6"/>
     </row>
     <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2022</v>
       </c>
       <c r="B20" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C20" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="F20" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
       </c>
-      <c r="L20" s="6" t="s">
-        <v>45</v>
+      <c r="L20" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M20" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N20" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O20" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O20" s="6"/>
     </row>
     <row r="21" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2022</v>
       </c>
       <c r="B21" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C21" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K21" s="2">
         <v>0</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>45</v>
+      <c r="L21" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M21" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N21" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O21" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O21" s="6"/>
     </row>
     <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2022</v>
       </c>
       <c r="B22" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C22" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K22" s="2">
         <v>0</v>
       </c>
-      <c r="L22" s="6" t="s">
-        <v>45</v>
+      <c r="L22" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M22" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N22" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O22" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O22" s="6"/>
     </row>
     <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2022</v>
       </c>
       <c r="B23" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C23" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K23" s="2">
         <v>0</v>
       </c>
-      <c r="L23" s="6" t="s">
-        <v>45</v>
+      <c r="L23" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M23" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N23" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O23" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O23" s="6"/>
     </row>
     <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2022</v>
       </c>
       <c r="B24" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C24" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K24" s="2">
         <v>0</v>
       </c>
-      <c r="L24" s="6" t="s">
-        <v>45</v>
+      <c r="L24" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M24" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N24" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O24" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O24" s="6"/>
     </row>
     <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2022</v>
       </c>
       <c r="B25" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C25" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
       </c>
-      <c r="L25" s="6" t="s">
-        <v>45</v>
+      <c r="L25" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M25" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N25" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O25" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O25" s="6"/>
     </row>
     <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2022</v>
       </c>
       <c r="B26" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C26" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K26" s="2">
         <v>0</v>
       </c>
-      <c r="L26" s="6" t="s">
-        <v>45</v>
+      <c r="L26" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M26" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N26" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O26" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O26" s="6"/>
     </row>
     <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2022</v>
       </c>
       <c r="B27" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C27" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K27" s="2">
         <v>0</v>
       </c>
-      <c r="L27" s="6" t="s">
-        <v>45</v>
+      <c r="L27" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M27" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N27" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O27" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O27" s="6"/>
     </row>
     <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2022</v>
       </c>
       <c r="B28" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C28" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
       </c>
-      <c r="L28" s="6" t="s">
-        <v>45</v>
+      <c r="L28" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M28" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N28" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O28" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O28" s="6"/>
     </row>
     <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2022</v>
       </c>
       <c r="B29" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C29" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K29" s="2">
         <v>0</v>
       </c>
-      <c r="L29" s="6" t="s">
-        <v>45</v>
+      <c r="L29" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M29" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N29" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O29" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O29" s="6"/>
     </row>
     <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>2022</v>
       </c>
       <c r="B30" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C30" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K30" s="2">
         <v>0</v>
       </c>
-      <c r="L30" s="6" t="s">
-        <v>45</v>
+      <c r="L30" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M30" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N30" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O30" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>2022</v>
       </c>
       <c r="B31" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C31" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K31" s="2">
         <v>0</v>
       </c>
-      <c r="L31" s="6" t="s">
-        <v>45</v>
+      <c r="L31" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M31" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N31" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O31" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O31" s="6"/>
     </row>
     <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>2022</v>
       </c>
       <c r="B32" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C32" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F32" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="H32" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
       </c>
-      <c r="L32" s="6" t="s">
-        <v>45</v>
+      <c r="L32" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M32" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N32" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O32" s="7"/>
-    </row>
-    <row r="33" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2022</v>
       </c>
       <c r="B33" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C33" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
       </c>
-      <c r="L33" s="6" t="s">
-        <v>45</v>
+      <c r="L33" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M33" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N33" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O33" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O33" s="6"/>
     </row>
     <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>2022</v>
       </c>
       <c r="B34" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C34" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K34" s="2">
         <v>0</v>
       </c>
-      <c r="L34" s="6" t="s">
-        <v>45</v>
+      <c r="L34" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M34" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N34" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O34" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O34" s="6"/>
     </row>
     <row r="35" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>2022</v>
       </c>
       <c r="B35" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C35" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K35" s="2">
         <v>0</v>
       </c>
-      <c r="L35" s="6" t="s">
-        <v>45</v>
+      <c r="L35" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M35" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N35" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O35" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O35" s="6"/>
     </row>
     <row r="36" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>2022</v>
       </c>
       <c r="B36" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C36" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K36" s="2">
         <v>0</v>
       </c>
-      <c r="L36" s="6" t="s">
-        <v>45</v>
+      <c r="L36" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M36" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N36" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O36" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O36" s="6"/>
     </row>
     <row r="37" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2022</v>
       </c>
       <c r="B37" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C37" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F37" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="H37" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K37" s="2">
         <v>0</v>
       </c>
-      <c r="L37" s="6" t="s">
-        <v>45</v>
+      <c r="L37" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M37" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N37" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O37" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O37" s="6"/>
     </row>
     <row r="38" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2022</v>
       </c>
       <c r="B38" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C38" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K38" s="2">
         <v>0</v>
       </c>
-      <c r="L38" s="6" t="s">
-        <v>45</v>
+      <c r="L38" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M38" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N38" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O38" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O38" s="6"/>
     </row>
     <row r="39" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2022</v>
       </c>
       <c r="B39" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C39" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D39" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="F39" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K39" s="2">
         <v>0</v>
       </c>
-      <c r="L39" s="6" t="s">
-        <v>45</v>
+      <c r="L39" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M39" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N39" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O39" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O39" s="6"/>
     </row>
     <row r="40" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2022</v>
       </c>
       <c r="B40" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C40" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K40" s="2">
         <v>0</v>
       </c>
-      <c r="L40" s="6" t="s">
-        <v>45</v>
+      <c r="L40" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M40" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N40" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O40" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O40" s="6"/>
     </row>
     <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2022</v>
       </c>
       <c r="B41" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C41" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K41" s="2">
         <v>0</v>
       </c>
-      <c r="L41" s="6" t="s">
-        <v>45</v>
+      <c r="L41" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M41" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N41" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O41" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O41" s="6"/>
     </row>
     <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>2022</v>
       </c>
       <c r="B42" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C42" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K42" s="2">
         <v>0</v>
       </c>
-      <c r="L42" s="6" t="s">
-        <v>45</v>
+      <c r="L42" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M42" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N42" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O42" s="7"/>
-    </row>
-    <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>2022</v>
       </c>
       <c r="B43" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C43" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
       </c>
-      <c r="L43" s="6" t="s">
-        <v>45</v>
+      <c r="L43" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M43" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N43" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O43" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O43" s="6"/>
     </row>
     <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>2022</v>
       </c>
       <c r="B44" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C44" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K44" s="2">
         <v>0</v>
       </c>
-      <c r="L44" s="6" t="s">
-        <v>45</v>
+      <c r="L44" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M44" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N44" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O44" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O44" s="6"/>
     </row>
     <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>2022</v>
       </c>
       <c r="B45" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C45" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K45" s="2">
         <v>0</v>
       </c>
-      <c r="L45" s="6" t="s">
-        <v>45</v>
+      <c r="L45" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M45" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N45" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O45" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O45" s="6"/>
     </row>
     <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>2022</v>
       </c>
       <c r="B46" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C46" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K46" s="2">
         <v>0</v>
       </c>
-      <c r="L46" s="6" t="s">
-        <v>45</v>
+      <c r="L46" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M46" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N46" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O46" s="7"/>
-    </row>
-    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>2022</v>
       </c>
       <c r="B47" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C47" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K47" s="2">
         <v>0</v>
       </c>
-      <c r="L47" s="6" t="s">
-        <v>45</v>
+      <c r="L47" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M47" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N47" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O47" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O47" s="6"/>
     </row>
     <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>2022</v>
       </c>
       <c r="B48" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C48" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K48" s="2">
         <v>0</v>
       </c>
-      <c r="L48" s="6" t="s">
-        <v>45</v>
+      <c r="L48" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M48" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N48" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O48" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O48" s="6"/>
     </row>
     <row r="49" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>2022</v>
       </c>
       <c r="B49" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C49" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K49" s="2">
         <v>0</v>
       </c>
-      <c r="L49" s="6" t="s">
-        <v>45</v>
+      <c r="L49" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M49" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N49" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O49" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O49" s="6"/>
     </row>
     <row r="50" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>2022</v>
       </c>
       <c r="B50" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C50" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K50" s="2">
         <v>0</v>
       </c>
-      <c r="L50" s="6" t="s">
-        <v>45</v>
+      <c r="L50" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M50" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N50" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O50" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O50" s="6"/>
     </row>
     <row r="51" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>2022</v>
       </c>
       <c r="B51" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C51" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K51" s="2">
         <v>0</v>
       </c>
-      <c r="L51" s="6" t="s">
-        <v>45</v>
+      <c r="L51" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M51" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N51" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O51" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O51" s="6"/>
     </row>
     <row r="52" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>2022</v>
       </c>
       <c r="B52" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C52" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K52" s="2">
         <v>0</v>
       </c>
-      <c r="L52" s="6" t="s">
-        <v>45</v>
+      <c r="L52" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M52" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N52" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O52" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O52" s="6"/>
     </row>
     <row r="53" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2022</v>
       </c>
       <c r="B53" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C53" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K53" s="2">
         <v>0</v>
       </c>
-      <c r="L53" s="6" t="s">
-        <v>45</v>
+      <c r="L53" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M53" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N53" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O53" s="7"/>
-    </row>
-    <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O53" s="6"/>
+    </row>
+    <row r="54" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>2022</v>
       </c>
       <c r="B54" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C54" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K54" s="2">
         <v>0</v>
       </c>
-      <c r="L54" s="6" t="s">
-        <v>45</v>
+      <c r="L54" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M54" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N54" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O54" s="7"/>
-    </row>
-    <row r="55" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O54" s="6"/>
+    </row>
+    <row r="55" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>2022</v>
       </c>
       <c r="B55" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C55" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K55" s="2">
         <v>0</v>
       </c>
-      <c r="L55" s="6" t="s">
-        <v>45</v>
+      <c r="L55" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M55" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N55" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O55" s="7"/>
-    </row>
-    <row r="56" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O55" s="6"/>
+    </row>
+    <row r="56" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>2022</v>
       </c>
       <c r="B56" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C56" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K56" s="2">
         <v>0</v>
       </c>
-      <c r="L56" s="6" t="s">
-        <v>45</v>
+      <c r="L56" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M56" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N56" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O56" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O56" s="6"/>
     </row>
     <row r="57" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>2022</v>
       </c>
       <c r="B57" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C57" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K57" s="2">
         <v>0</v>
       </c>
-      <c r="L57" s="6" t="s">
-        <v>45</v>
+      <c r="L57" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M57" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N57" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O57" s="7"/>
-    </row>
-    <row r="58" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44844</v>
+      </c>
+      <c r="O57" s="6"/>
+    </row>
+    <row r="58" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>2022</v>
       </c>
       <c r="B58" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C58" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K58" s="2">
         <v>0</v>
       </c>
-      <c r="L58" s="6" t="s">
-        <v>45</v>
+      <c r="L58" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M58" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N58" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O58" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O58" s="6"/>
     </row>
     <row r="59" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>2022</v>
       </c>
       <c r="B59" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C59" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K59" s="2">
         <v>0</v>
       </c>
-      <c r="L59" s="6" t="s">
-        <v>45</v>
+      <c r="L59" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M59" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N59" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O59" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O59" s="6"/>
     </row>
     <row r="60" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>2022</v>
       </c>
       <c r="B60" s="3">
-        <v>44652</v>
+        <v>44743</v>
       </c>
       <c r="C60" s="3">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K60" s="2">
         <v>0</v>
       </c>
-      <c r="L60" s="6" t="s">
-        <v>45</v>
+      <c r="L60" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="M60" s="3">
-        <v>44753</v>
+        <v>44844</v>
       </c>
       <c r="N60" s="3">
-        <v>44753</v>
-      </c>
-      <c r="O60" s="7"/>
+        <v>44844</v>
+      </c>
+      <c r="O60" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3656,6 +3654,6 @@
     <hyperlink ref="J12" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
</xml_diff>